<commit_message>
finish first version of pic
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mycode\emer-testbed\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A41FB44-184E-4110-97CC-AF85C94E23C5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70752751-63BB-4FE5-A283-78707DE75DB5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="12708" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1212,7 +1212,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1259,8 +1259,8 @@
         <v>50</v>
       </c>
       <c r="L2">
-        <f>2.541579*15813/(3500/K2)</f>
-        <v>574.14269610000008</v>
+        <f>2.541579*2233/(3500/K2)</f>
+        <v>81.076370100000005</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1285,8 +1285,8 @@
         <v>100</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L8" si="1">2.541579*15813/(3500/K3)</f>
-        <v>1148.2853922000002</v>
+        <f t="shared" ref="L3:L8" si="1">2.541579*2233/(3500/K3)</f>
+        <v>162.15274020000001</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
-        <v>2296.5707844000003</v>
+        <v>324.30548040000002</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>2870.7134805000001</v>
+        <v>405.38185049999998</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>3444.8561766000003</v>
+        <v>486.4582206</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
-        <v>4018.9988727000004</v>
+        <v>567.53459069999997</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1404,7 +1404,7 @@
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>4593.1415688000006</v>
+        <v>648.61096080000004</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="57.6">
@@ -1427,8 +1427,8 @@
         <v>50</v>
       </c>
       <c r="L9">
-        <f>3*1.4+15813*1.143/(3500/K9)</f>
-        <v>262.40370000000001</v>
+        <f>3*1.4+2233*1.143/(3500/K9)</f>
+        <v>40.661699999999996</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1448,8 +1448,8 @@
         <v>100</v>
       </c>
       <c r="L10">
-        <f t="shared" ref="L10:L22" si="4">3*1.4+15813*1.143/(3500/K10)</f>
-        <v>520.6074000000001</v>
+        <f t="shared" ref="L10:L15" si="4">3*1.4+2233*1.143/(3500/K10)</f>
+        <v>77.123400000000004</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="L11">
         <f t="shared" si="4"/>
-        <v>1037.0148000000002</v>
+        <v>150.04679999999999</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="L12">
         <f t="shared" si="4"/>
-        <v>1295.2185000000002</v>
+        <v>186.5085</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="L13">
         <f t="shared" si="4"/>
-        <v>1553.4222000000002</v>
+        <v>222.97020000000001</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="L14">
         <f t="shared" si="4"/>
-        <v>1811.6259000000002</v>
+        <v>259.43189999999998</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1554,7 +1554,7 @@
       </c>
       <c r="L15">
         <f t="shared" si="4"/>
-        <v>2069.8296</v>
+        <v>295.89359999999999</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1563,8 +1563,8 @@
         <v>50</v>
       </c>
       <c r="L16">
-        <f>3*1.4+(15813-3671)*1.143/(3500/K16)</f>
-        <v>202.46151428571429</v>
+        <f>3*1.4+(2233-517)*1.143/(3500/K16)</f>
+        <v>32.219828571428565</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1573,8 +1573,8 @@
         <v>100</v>
       </c>
       <c r="L17">
-        <f t="shared" ref="L17:L22" si="5">3*1.4+(15813-3671)*1.143/(3500/K17)</f>
-        <v>400.72302857142859</v>
+        <f t="shared" ref="L17:L22" si="5">3*1.4+(2233-517)*1.143/(3500/K17)</f>
+        <v>60.239657142857141</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="L18">
         <f t="shared" si="5"/>
-        <v>797.24605714285724</v>
+        <v>116.27931428571428</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1594,7 +1594,7 @@
       </c>
       <c r="L19">
         <f t="shared" si="5"/>
-        <v>995.50757142857151</v>
+        <v>144.29914285714284</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="L20">
         <f t="shared" si="5"/>
-        <v>1193.7690857142859</v>
+        <v>172.31897142857142</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="L21">
         <f t="shared" si="5"/>
-        <v>1392.0306</v>
+        <v>200.33879999999999</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1624,7 +1624,7 @@
       </c>
       <c r="L22">
         <f t="shared" si="5"/>
-        <v>1590.2921142857144</v>
+        <v>228.35862857142854</v>
       </c>
     </row>
     <row r="23" spans="1:12">

</xml_diff>

<commit_message>
create a new chart graph1-3
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mycode\emer-testbed\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70752751-63BB-4FE5-A283-78707DE75DB5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D964A0-6DD5-4804-BD29-DC2FB8A4631A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="12708" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="12708" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -702,7 +702,7 @@
       <c r="D6">
         <v>1000</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>1500</v>
       </c>
       <c r="F6">
@@ -722,11 +722,13 @@
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
         <v>0</v>
       </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
@@ -738,7 +740,7 @@
       <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F9" t="s">
@@ -764,7 +766,7 @@
       <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F10" t="s">
@@ -816,7 +818,7 @@
       <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F12" t="s">
@@ -842,7 +844,7 @@
       <c r="D13" t="s">
         <v>36</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F13" t="s">
@@ -868,7 +870,7 @@
       <c r="D14" t="s">
         <v>43</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F14" t="s">
@@ -894,7 +896,7 @@
       <c r="D15" t="s">
         <v>50</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F15" t="s">
@@ -920,7 +922,7 @@
       <c r="D16" t="s">
         <v>57</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F16" t="s">
@@ -1211,7 +1213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557FBDEE-5A86-4FBF-82C5-EC2A93BC7B31}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>

</xml_diff>